<commit_message>
Remove Tuple To Alias Table
</commit_message>
<xml_diff>
--- a/Demo/Data/0_no_loc/data/Item.xlsx
+++ b/Demo/Data/0_no_loc/data/Item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fancyHub\ExportExcel\Demo\Data\0_no_loc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE775A35-A053-46EF-AC8D-6C36567DC888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29C23FE-FFA4-4980-82C9-7E1D19CE34A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>#remark</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -263,16 +263,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>int_bool
-TupleAlias[PairItemIntBool]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>list_int_int64
-TupleAlias[PairItemIntInt64]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>PairField2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -293,11 +283,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>int_int
-TupleAlias[PairItemIntBool]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1|3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -323,6 +308,36 @@
   </si>
   <si>
     <t>紫色</t>
+  </si>
+  <si>
+    <t>EnumFieldName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnumName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExcelVal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Val</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">int_bool
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>int_int</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">list_int_int64
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -799,11 +814,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -842,16 +857,16 @@
         <v>48</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>49</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>50</v>
@@ -875,19 +890,19 @@
         <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>51</v>
@@ -946,7 +961,7 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>53</v>
@@ -955,7 +970,7 @@
         <v>53</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
         <v>54</v>
@@ -1037,28 +1052,28 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1114,9 +1129,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBBD7ED-714C-4183-A67A-A09FF8ED8A63}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1250,7 +1265,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>25</v>
@@ -1265,13 +1280,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D12" s="8">
         <v>1</v>
@@ -1280,13 +1295,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="C13" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="8">
         <v>2</v>

</xml_diff>